<commit_message>
Update totalorcadofrotas.xlsx and frota_llm/frota.db
</commit_message>
<xml_diff>
--- a/apps/linux/frota_etl/totalorcadofrotas.xlsx
+++ b/apps/linux/frota_etl/totalorcadofrotas.xlsx
@@ -1133,48 +1133,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1414,7 +1410,7 @@
   </sheetPr>
   <dimension ref="A1:AL673"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
     </sheetView>
   </sheetViews>
@@ -40178,13 +40174,13 @@
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="3" t="n">
-        <v>5213</v>
+        <v>4215</v>
       </c>
       <c r="B306" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C306" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D306" s="3" t="s">
         <v>55</v>
@@ -40213,14 +40209,14 @@
         <v>0</v>
       </c>
       <c r="L306" s="5" t="n">
-        <v>18968.04</v>
+        <v>30693.44</v>
       </c>
       <c r="M306" s="6" t="n">
-        <v>2850.28</v>
+        <v>6302.883</v>
       </c>
       <c r="N306" s="7" t="n">
         <f aca="false">M306-L306</f>
-        <v>-16117.76</v>
+        <v>-24390.557</v>
       </c>
       <c r="O306" s="5" t="n">
         <v>0</v>
@@ -40276,42 +40272,42 @@
         <v>0</v>
       </c>
       <c r="AE306" s="6" t="n">
-        <v>24.43</v>
+        <v>121.543</v>
       </c>
       <c r="AF306" s="7" t="n">
         <f aca="false">AE306-AD306</f>
-        <v>24.43</v>
+        <v>121.543</v>
       </c>
       <c r="AG306" s="5" t="n">
-        <v>18968.04</v>
+        <v>20693.44</v>
       </c>
       <c r="AH306" s="6" t="n">
-        <v>2825.85</v>
+        <v>3962.51</v>
       </c>
       <c r="AI306" s="7" t="n">
         <f aca="false">AH306-AG306</f>
-        <v>-16142.19</v>
+        <v>-16730.93</v>
       </c>
       <c r="AJ306" s="5" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="AK306" s="6" t="n">
-        <v>0</v>
+        <v>2218.83</v>
       </c>
       <c r="AL306" s="7" t="n">
         <f aca="false">AK306-AJ306</f>
-        <v>0</v>
+        <v>-7781.17</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="3" t="n">
-        <v>5216</v>
+        <v>5213</v>
       </c>
       <c r="B307" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C307" s="3" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="D307" s="3" t="s">
         <v>55</v>
@@ -40340,14 +40336,14 @@
         <v>0</v>
       </c>
       <c r="L307" s="5" t="n">
-        <v>12532.64</v>
+        <v>18968.04</v>
       </c>
       <c r="M307" s="6" t="n">
-        <v>98716.891</v>
+        <v>2850.28</v>
       </c>
       <c r="N307" s="7" t="n">
         <f aca="false">M307-L307</f>
-        <v>86184.251</v>
+        <v>-16117.76</v>
       </c>
       <c r="O307" s="5" t="n">
         <v>0</v>
@@ -40383,11 +40379,11 @@
         <v>0</v>
       </c>
       <c r="Y307" s="6" t="n">
-        <v>2365.04</v>
+        <v>0</v>
       </c>
       <c r="Z307" s="7" t="n">
         <f aca="false">Y307-X307</f>
-        <v>2365.04</v>
+        <v>0</v>
       </c>
       <c r="AA307" s="5" t="n">
         <v>0</v>
@@ -40403,21 +40399,21 @@
         <v>0</v>
       </c>
       <c r="AE307" s="6" t="n">
-        <v>147.171</v>
+        <v>24.43</v>
       </c>
       <c r="AF307" s="7" t="n">
         <f aca="false">AE307-AD307</f>
-        <v>147.171</v>
+        <v>24.43</v>
       </c>
       <c r="AG307" s="5" t="n">
-        <v>12532.64</v>
+        <v>18968.04</v>
       </c>
       <c r="AH307" s="6" t="n">
-        <v>96204.68</v>
+        <v>2825.85</v>
       </c>
       <c r="AI307" s="7" t="n">
         <f aca="false">AH307-AG307</f>
-        <v>83672.04</v>
+        <v>-16142.19</v>
       </c>
       <c r="AJ307" s="5" t="n">
         <v>0</v>
@@ -40432,13 +40428,13 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="3" t="n">
-        <v>4216</v>
+        <v>5216</v>
       </c>
       <c r="B308" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C308" s="3" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="D308" s="3" t="s">
         <v>55</v>
@@ -40467,14 +40463,14 @@
         <v>0</v>
       </c>
       <c r="L308" s="5" t="n">
-        <v>17110.54</v>
+        <v>12532.64</v>
       </c>
       <c r="M308" s="6" t="n">
-        <v>14301.676</v>
+        <v>98716.891</v>
       </c>
       <c r="N308" s="7" t="n">
         <f aca="false">M308-L308</f>
-        <v>-2808.864</v>
+        <v>86184.251</v>
       </c>
       <c r="O308" s="5" t="n">
         <v>0</v>
@@ -40510,11 +40506,11 @@
         <v>0</v>
       </c>
       <c r="Y308" s="6" t="n">
-        <v>3187.668</v>
+        <v>2365.04</v>
       </c>
       <c r="Z308" s="7" t="n">
         <f aca="false">Y308-X308</f>
-        <v>3187.668</v>
+        <v>2365.04</v>
       </c>
       <c r="AA308" s="5" t="n">
         <v>0</v>
@@ -40530,21 +40526,21 @@
         <v>0</v>
       </c>
       <c r="AE308" s="6" t="n">
-        <v>84.058</v>
+        <v>147.171</v>
       </c>
       <c r="AF308" s="7" t="n">
         <f aca="false">AE308-AD308</f>
-        <v>84.058</v>
+        <v>147.171</v>
       </c>
       <c r="AG308" s="5" t="n">
-        <v>17110.54</v>
+        <v>12532.64</v>
       </c>
       <c r="AH308" s="6" t="n">
-        <v>11029.95</v>
+        <v>96204.68</v>
       </c>
       <c r="AI308" s="7" t="n">
         <f aca="false">AH308-AG308</f>
-        <v>-6080.59</v>
+        <v>83672.04</v>
       </c>
       <c r="AJ308" s="5" t="n">
         <v>0</v>
@@ -40559,13 +40555,13 @@
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="3" t="n">
-        <v>8221</v>
+        <v>4216</v>
       </c>
       <c r="B309" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C309" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D309" s="3" t="s">
         <v>55</v>
@@ -40594,14 +40590,14 @@
         <v>0</v>
       </c>
       <c r="L309" s="5" t="n">
-        <v>121819.85</v>
+        <v>17110.54</v>
       </c>
       <c r="M309" s="6" t="n">
-        <v>407668.355</v>
+        <v>14301.676</v>
       </c>
       <c r="N309" s="7" t="n">
         <f aca="false">M309-L309</f>
-        <v>285848.505</v>
+        <v>-2808.864</v>
       </c>
       <c r="O309" s="5" t="n">
         <v>0</v>
@@ -40637,11 +40633,11 @@
         <v>0</v>
       </c>
       <c r="Y309" s="6" t="n">
-        <v>17993.11</v>
+        <v>3187.668</v>
       </c>
       <c r="Z309" s="7" t="n">
         <f aca="false">Y309-X309</f>
-        <v>17993.11</v>
+        <v>3187.668</v>
       </c>
       <c r="AA309" s="5" t="n">
         <v>0</v>
@@ -40657,42 +40653,42 @@
         <v>0</v>
       </c>
       <c r="AE309" s="6" t="n">
-        <v>267.705</v>
+        <v>84.058</v>
       </c>
       <c r="AF309" s="7" t="n">
         <f aca="false">AE309-AD309</f>
-        <v>267.705</v>
+        <v>84.058</v>
       </c>
       <c r="AG309" s="5" t="n">
-        <v>61819.85</v>
+        <v>17110.54</v>
       </c>
       <c r="AH309" s="6" t="n">
-        <v>95067.19</v>
+        <v>11029.95</v>
       </c>
       <c r="AI309" s="7" t="n">
         <f aca="false">AH309-AG309</f>
-        <v>33247.34</v>
+        <v>-6080.59</v>
       </c>
       <c r="AJ309" s="5" t="n">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="AK309" s="6" t="n">
-        <v>294340.35</v>
+        <v>0</v>
       </c>
       <c r="AL309" s="7" t="n">
         <f aca="false">AK309-AJ309</f>
-        <v>234340.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="3" t="n">
-        <v>222</v>
+        <v>8221</v>
       </c>
       <c r="B310" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C310" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D310" s="3" t="s">
         <v>55</v>
@@ -40721,14 +40717,14 @@
         <v>0</v>
       </c>
       <c r="L310" s="5" t="n">
-        <v>119766.15</v>
+        <v>121819.85</v>
       </c>
       <c r="M310" s="6" t="n">
-        <v>220827.516</v>
+        <v>407668.355</v>
       </c>
       <c r="N310" s="7" t="n">
         <f aca="false">M310-L310</f>
-        <v>101061.366</v>
+        <v>285848.505</v>
       </c>
       <c r="O310" s="5" t="n">
         <v>0</v>
@@ -40764,11 +40760,11 @@
         <v>0</v>
       </c>
       <c r="Y310" s="6" t="n">
-        <v>4208.775</v>
+        <v>17993.11</v>
       </c>
       <c r="Z310" s="7" t="n">
         <f aca="false">Y310-X310</f>
-        <v>4208.775</v>
+        <v>17993.11</v>
       </c>
       <c r="AA310" s="5" t="n">
         <v>0</v>
@@ -40784,42 +40780,42 @@
         <v>0</v>
       </c>
       <c r="AE310" s="6" t="n">
-        <v>1041.741</v>
+        <v>267.705</v>
       </c>
       <c r="AF310" s="7" t="n">
         <f aca="false">AE310-AD310</f>
-        <v>1041.741</v>
+        <v>267.705</v>
       </c>
       <c r="AG310" s="5" t="n">
-        <v>119766.15</v>
+        <v>61819.85</v>
       </c>
       <c r="AH310" s="6" t="n">
-        <v>215577</v>
+        <v>95067.19</v>
       </c>
       <c r="AI310" s="7" t="n">
         <f aca="false">AH310-AG310</f>
-        <v>95810.85</v>
+        <v>33247.34</v>
       </c>
       <c r="AJ310" s="5" t="n">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="AK310" s="6" t="n">
-        <v>0</v>
+        <v>294340.35</v>
       </c>
       <c r="AL310" s="7" t="n">
         <f aca="false">AK310-AJ310</f>
-        <v>0</v>
+        <v>234340.35</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="3" t="n">
-        <v>2815</v>
+        <v>222</v>
       </c>
       <c r="B311" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C311" s="3" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="D311" s="3" t="s">
         <v>55</v>
@@ -40848,14 +40844,14 @@
         <v>0</v>
       </c>
       <c r="L311" s="5" t="n">
-        <v>26622.92</v>
+        <v>119766.15</v>
       </c>
       <c r="M311" s="6" t="n">
-        <v>11032.3917</v>
+        <v>220827.516</v>
       </c>
       <c r="N311" s="7" t="n">
         <f aca="false">M311-L311</f>
-        <v>-15590.5283</v>
+        <v>101061.366</v>
       </c>
       <c r="O311" s="5" t="n">
         <v>0</v>
@@ -40891,11 +40887,11 @@
         <v>0</v>
       </c>
       <c r="Y311" s="6" t="n">
-        <v>0</v>
+        <v>4208.775</v>
       </c>
       <c r="Z311" s="7" t="n">
         <f aca="false">Y311-X311</f>
-        <v>0</v>
+        <v>4208.775</v>
       </c>
       <c r="AA311" s="5" t="n">
         <v>0</v>
@@ -40911,42 +40907,42 @@
         <v>0</v>
       </c>
       <c r="AE311" s="6" t="n">
-        <v>231.9417</v>
+        <v>1041.741</v>
       </c>
       <c r="AF311" s="7" t="n">
         <f aca="false">AE311-AD311</f>
-        <v>231.9417</v>
+        <v>1041.741</v>
       </c>
       <c r="AG311" s="5" t="n">
-        <v>16622.92</v>
+        <v>119766.15</v>
       </c>
       <c r="AH311" s="6" t="n">
-        <v>10800.45</v>
+        <v>215577</v>
       </c>
       <c r="AI311" s="7" t="n">
         <f aca="false">AH311-AG311</f>
-        <v>-5822.47</v>
+        <v>95810.85</v>
       </c>
       <c r="AJ311" s="5" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="AK311" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL311" s="7" t="n">
         <f aca="false">AK311-AJ311</f>
-        <v>-10000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="3" t="n">
-        <v>1815</v>
+        <v>2815</v>
       </c>
       <c r="B312" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C312" s="3" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="D312" s="3" t="s">
         <v>55</v>
@@ -40975,14 +40971,14 @@
         <v>0</v>
       </c>
       <c r="L312" s="5" t="n">
-        <v>5000</v>
+        <v>26622.92</v>
       </c>
       <c r="M312" s="6" t="n">
-        <v>28561.5365</v>
+        <v>11032.3917</v>
       </c>
       <c r="N312" s="7" t="n">
         <f aca="false">M312-L312</f>
-        <v>23561.5365</v>
+        <v>-15590.5283</v>
       </c>
       <c r="O312" s="5" t="n">
         <v>0</v>
@@ -41038,42 +41034,42 @@
         <v>0</v>
       </c>
       <c r="AE312" s="6" t="n">
-        <v>136.0965</v>
+        <v>231.9417</v>
       </c>
       <c r="AF312" s="7" t="n">
         <f aca="false">AE312-AD312</f>
-        <v>136.0965</v>
+        <v>231.9417</v>
       </c>
       <c r="AG312" s="5" t="n">
-        <v>5000</v>
+        <v>16622.92</v>
       </c>
       <c r="AH312" s="6" t="n">
-        <v>4440.89</v>
+        <v>10800.45</v>
       </c>
       <c r="AI312" s="7" t="n">
         <f aca="false">AH312-AG312</f>
-        <v>-559.11</v>
+        <v>-5822.47</v>
       </c>
       <c r="AJ312" s="5" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="AK312" s="6" t="n">
-        <v>23984.55</v>
+        <v>0</v>
       </c>
       <c r="AL312" s="7" t="n">
         <f aca="false">AK312-AJ312</f>
-        <v>23984.55</v>
+        <v>-10000</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="3" t="n">
-        <v>4315</v>
+        <v>1815</v>
       </c>
       <c r="B313" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C313" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D313" s="3" t="s">
         <v>55</v>
@@ -41102,14 +41098,14 @@
         <v>0</v>
       </c>
       <c r="L313" s="5" t="n">
-        <v>4253.98</v>
+        <v>5000</v>
       </c>
       <c r="M313" s="6" t="n">
-        <v>6136.209</v>
+        <v>28561.5365</v>
       </c>
       <c r="N313" s="7" t="n">
         <f aca="false">M313-L313</f>
-        <v>1882.229</v>
+        <v>23561.5365</v>
       </c>
       <c r="O313" s="5" t="n">
         <v>0</v>
@@ -41165,42 +41161,42 @@
         <v>0</v>
       </c>
       <c r="AE313" s="6" t="n">
-        <v>20.749</v>
+        <v>136.0965</v>
       </c>
       <c r="AF313" s="7" t="n">
         <f aca="false">AE313-AD313</f>
-        <v>20.749</v>
+        <v>136.0965</v>
       </c>
       <c r="AG313" s="5" t="n">
-        <v>4253.98</v>
+        <v>5000</v>
       </c>
       <c r="AH313" s="6" t="n">
-        <v>6115.46</v>
+        <v>4440.89</v>
       </c>
       <c r="AI313" s="7" t="n">
         <f aca="false">AH313-AG313</f>
-        <v>1861.48</v>
+        <v>-559.11</v>
       </c>
       <c r="AJ313" s="5" t="n">
         <v>0</v>
       </c>
       <c r="AK313" s="6" t="n">
-        <v>0</v>
+        <v>23984.55</v>
       </c>
       <c r="AL313" s="7" t="n">
         <f aca="false">AK313-AJ313</f>
-        <v>0</v>
+        <v>23984.55</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="3" t="n">
-        <v>809</v>
+        <v>4315</v>
       </c>
       <c r="B314" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C314" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D314" s="3" t="s">
         <v>55</v>
@@ -41229,14 +41225,14 @@
         <v>0</v>
       </c>
       <c r="L314" s="5" t="n">
-        <v>0</v>
+        <v>4253.98</v>
       </c>
       <c r="M314" s="6" t="n">
-        <v>0</v>
+        <v>6136.209</v>
       </c>
       <c r="N314" s="7" t="n">
         <f aca="false">M314-L314</f>
-        <v>0</v>
+        <v>1882.229</v>
       </c>
       <c r="O314" s="5" t="n">
         <v>0</v>
@@ -41292,21 +41288,21 @@
         <v>0</v>
       </c>
       <c r="AE314" s="6" t="n">
-        <v>0</v>
+        <v>20.749</v>
       </c>
       <c r="AF314" s="7" t="n">
         <f aca="false">AE314-AD314</f>
-        <v>0</v>
+        <v>20.749</v>
       </c>
       <c r="AG314" s="5" t="n">
-        <v>0</v>
+        <v>4253.98</v>
       </c>
       <c r="AH314" s="6" t="n">
-        <v>0</v>
+        <v>6115.46</v>
       </c>
       <c r="AI314" s="7" t="n">
         <f aca="false">AH314-AG314</f>
-        <v>0</v>
+        <v>1861.48</v>
       </c>
       <c r="AJ314" s="5" t="n">
         <v>0</v>
@@ -41321,16 +41317,16 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="3" t="n">
-        <v>2224</v>
+        <v>809</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D315" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E315" s="3" t="s">
         <v>151</v>
@@ -41448,10 +41444,10 @@
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="3" t="n">
-        <v>1224</v>
+        <v>2224</v>
       </c>
       <c r="B316" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C316" s="3" t="s">
         <v>39</v>
@@ -41486,11 +41482,11 @@
         <v>0</v>
       </c>
       <c r="M316" s="6" t="n">
-        <v>1526</v>
+        <v>0</v>
       </c>
       <c r="N316" s="7" t="n">
         <f aca="false">M316-L316</f>
-        <v>1526</v>
+        <v>0</v>
       </c>
       <c r="O316" s="5" t="n">
         <v>0</v>
@@ -41556,11 +41552,11 @@
         <v>0</v>
       </c>
       <c r="AH316" s="6" t="n">
-        <v>1526</v>
+        <v>0</v>
       </c>
       <c r="AI316" s="7" t="n">
         <f aca="false">AH316-AG316</f>
-        <v>1526</v>
+        <v>0</v>
       </c>
       <c r="AJ316" s="5" t="n">
         <v>0</v>
@@ -41575,16 +41571,16 @@
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="3" t="n">
-        <v>200</v>
+        <v>1224</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C317" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D317" s="3" t="s">
-        <v>176</v>
+        <v>65</v>
       </c>
       <c r="E317" s="3" t="s">
         <v>151</v>
@@ -41610,14 +41606,14 @@
         <v>0</v>
       </c>
       <c r="L317" s="5" t="n">
-        <v>1666.7</v>
+        <v>0</v>
       </c>
       <c r="M317" s="6" t="n">
-        <v>6624.18</v>
+        <v>1526</v>
       </c>
       <c r="N317" s="7" t="n">
         <f aca="false">M317-L317</f>
-        <v>4957.48</v>
+        <v>1526</v>
       </c>
       <c r="O317" s="5" t="n">
         <v>0</v>
@@ -41680,14 +41676,14 @@
         <v>0</v>
       </c>
       <c r="AG317" s="5" t="n">
-        <v>1666.7</v>
+        <v>0</v>
       </c>
       <c r="AH317" s="6" t="n">
-        <v>6624.18</v>
+        <v>1526</v>
       </c>
       <c r="AI317" s="7" t="n">
         <f aca="false">AH317-AG317</f>
-        <v>4957.48</v>
+        <v>1526</v>
       </c>
       <c r="AJ317" s="5" t="n">
         <v>0</v>
@@ -41702,13 +41698,13 @@
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="3" t="n">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B318" s="4" t="s">
         <v>200</v>
       </c>
       <c r="C318" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D318" s="3" t="s">
         <v>176</v>
@@ -41737,14 +41733,14 @@
         <v>0</v>
       </c>
       <c r="L318" s="5" t="n">
-        <v>16694.26</v>
+        <v>1666.7</v>
       </c>
       <c r="M318" s="6" t="n">
-        <v>8457.8</v>
+        <v>6624.18</v>
       </c>
       <c r="N318" s="7" t="n">
         <f aca="false">M318-L318</f>
-        <v>-8236.46</v>
+        <v>4957.48</v>
       </c>
       <c r="O318" s="5" t="n">
         <v>0</v>
@@ -41807,29 +41803,29 @@
         <v>0</v>
       </c>
       <c r="AG318" s="5" t="n">
-        <v>7894.26</v>
+        <v>1666.7</v>
       </c>
       <c r="AH318" s="6" t="n">
-        <v>4975.58</v>
+        <v>6624.18</v>
       </c>
       <c r="AI318" s="7" t="n">
         <f aca="false">AH318-AG318</f>
-        <v>-2918.68</v>
+        <v>4957.48</v>
       </c>
       <c r="AJ318" s="5" t="n">
-        <v>8800</v>
+        <v>0</v>
       </c>
       <c r="AK318" s="6" t="n">
-        <v>3482.22</v>
+        <v>0</v>
       </c>
       <c r="AL318" s="7" t="n">
         <f aca="false">AK318-AJ318</f>
-        <v>-5317.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="3" t="n">
-        <v>297</v>
+        <v>208</v>
       </c>
       <c r="B319" s="4" t="s">
         <v>200</v>
@@ -41864,14 +41860,14 @@
         <v>0</v>
       </c>
       <c r="L319" s="5" t="n">
-        <v>16514.26</v>
+        <v>16694.26</v>
       </c>
       <c r="M319" s="6" t="n">
-        <v>14421.98</v>
+        <v>8457.8</v>
       </c>
       <c r="N319" s="7" t="n">
         <f aca="false">M319-L319</f>
-        <v>-2092.28</v>
+        <v>-8236.46</v>
       </c>
       <c r="O319" s="5" t="n">
         <v>0</v>
@@ -41927,36 +41923,36 @@
         <v>0</v>
       </c>
       <c r="AE319" s="6" t="n">
-        <v>196.4</v>
+        <v>0</v>
       </c>
       <c r="AF319" s="7" t="n">
         <f aca="false">AE319-AD319</f>
-        <v>196.4</v>
+        <v>0</v>
       </c>
       <c r="AG319" s="5" t="n">
-        <v>7714.26</v>
+        <v>7894.26</v>
       </c>
       <c r="AH319" s="6" t="n">
-        <v>2420.22</v>
+        <v>4975.58</v>
       </c>
       <c r="AI319" s="7" t="n">
         <f aca="false">AH319-AG319</f>
-        <v>-5294.04</v>
+        <v>-2918.68</v>
       </c>
       <c r="AJ319" s="5" t="n">
         <v>8800</v>
       </c>
       <c r="AK319" s="6" t="n">
-        <v>11805.36</v>
+        <v>3482.22</v>
       </c>
       <c r="AL319" s="7" t="n">
         <f aca="false">AK319-AJ319</f>
-        <v>3005.36</v>
+        <v>-5317.78</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="3" t="n">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B320" s="4" t="s">
         <v>200</v>
@@ -41991,14 +41987,14 @@
         <v>0</v>
       </c>
       <c r="L320" s="5" t="n">
-        <v>21346.66</v>
+        <v>16514.26</v>
       </c>
       <c r="M320" s="6" t="n">
-        <v>25892.08</v>
+        <v>14421.98</v>
       </c>
       <c r="N320" s="7" t="n">
         <f aca="false">M320-L320</f>
-        <v>4545.42</v>
+        <v>-2092.28</v>
       </c>
       <c r="O320" s="5" t="n">
         <v>0</v>
@@ -42054,42 +42050,42 @@
         <v>0</v>
       </c>
       <c r="AE320" s="6" t="n">
-        <v>0</v>
+        <v>196.4</v>
       </c>
       <c r="AF320" s="7" t="n">
         <f aca="false">AE320-AD320</f>
-        <v>0</v>
+        <v>196.4</v>
       </c>
       <c r="AG320" s="5" t="n">
-        <v>12546.66</v>
+        <v>7714.26</v>
       </c>
       <c r="AH320" s="6" t="n">
-        <v>13910.15</v>
+        <v>2420.22</v>
       </c>
       <c r="AI320" s="7" t="n">
         <f aca="false">AH320-AG320</f>
-        <v>1363.49</v>
+        <v>-5294.04</v>
       </c>
       <c r="AJ320" s="5" t="n">
         <v>8800</v>
       </c>
       <c r="AK320" s="6" t="n">
-        <v>11981.93</v>
+        <v>11805.36</v>
       </c>
       <c r="AL320" s="7" t="n">
         <f aca="false">AK320-AJ320</f>
-        <v>3181.93</v>
+        <v>3005.36</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="3" t="n">
-        <v>4413</v>
+        <v>298</v>
       </c>
       <c r="B321" s="4" t="s">
         <v>200</v>
       </c>
       <c r="C321" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D321" s="3" t="s">
         <v>176</v>
@@ -42118,14 +42114,14 @@
         <v>0</v>
       </c>
       <c r="L321" s="5" t="n">
-        <v>29782</v>
+        <v>21346.66</v>
       </c>
       <c r="M321" s="6" t="n">
-        <v>27875.03</v>
+        <v>25892.08</v>
       </c>
       <c r="N321" s="7" t="n">
         <f aca="false">M321-L321</f>
-        <v>-1906.97</v>
+        <v>4545.42</v>
       </c>
       <c r="O321" s="5" t="n">
         <v>0</v>
@@ -42188,35 +42184,35 @@
         <v>0</v>
       </c>
       <c r="AG321" s="5" t="n">
-        <v>29782</v>
+        <v>12546.66</v>
       </c>
       <c r="AH321" s="6" t="n">
-        <v>27875.03</v>
+        <v>13910.15</v>
       </c>
       <c r="AI321" s="7" t="n">
         <f aca="false">AH321-AG321</f>
-        <v>-1906.97</v>
+        <v>1363.49</v>
       </c>
       <c r="AJ321" s="5" t="n">
-        <v>0</v>
+        <v>8800</v>
       </c>
       <c r="AK321" s="6" t="n">
-        <v>0</v>
+        <v>11981.93</v>
       </c>
       <c r="AL321" s="7" t="n">
         <f aca="false">AK321-AJ321</f>
-        <v>0</v>
+        <v>3181.93</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="3" t="n">
-        <v>7413</v>
+        <v>4413</v>
       </c>
       <c r="B322" s="4" t="s">
         <v>200</v>
       </c>
       <c r="C322" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D322" s="3" t="s">
         <v>176</v>
@@ -42245,14 +42241,14 @@
         <v>0</v>
       </c>
       <c r="L322" s="5" t="n">
-        <v>14622.58</v>
+        <v>29782</v>
       </c>
       <c r="M322" s="6" t="n">
-        <v>47948.11</v>
+        <v>27875.03</v>
       </c>
       <c r="N322" s="7" t="n">
         <f aca="false">M322-L322</f>
-        <v>33325.53</v>
+        <v>-1906.97</v>
       </c>
       <c r="O322" s="5" t="n">
         <v>0</v>
@@ -42308,21 +42304,21 @@
         <v>0</v>
       </c>
       <c r="AE322" s="6" t="n">
-        <v>252.92</v>
+        <v>0</v>
       </c>
       <c r="AF322" s="7" t="n">
         <f aca="false">AE322-AD322</f>
-        <v>252.92</v>
+        <v>0</v>
       </c>
       <c r="AG322" s="5" t="n">
-        <v>14622.58</v>
+        <v>29782</v>
       </c>
       <c r="AH322" s="6" t="n">
-        <v>47695.19</v>
+        <v>27875.03</v>
       </c>
       <c r="AI322" s="7" t="n">
         <f aca="false">AH322-AG322</f>
-        <v>33072.61</v>
+        <v>-1906.97</v>
       </c>
       <c r="AJ322" s="5" t="n">
         <v>0</v>
@@ -42337,10 +42333,10 @@
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="3" t="n">
-        <v>5210</v>
+        <v>7413</v>
       </c>
       <c r="B323" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C323" s="3" t="s">
         <v>45</v>
@@ -42372,14 +42368,14 @@
         <v>0</v>
       </c>
       <c r="L323" s="5" t="n">
-        <v>12500</v>
+        <v>14622.58</v>
       </c>
       <c r="M323" s="6" t="n">
-        <v>28070.22</v>
+        <v>47948.11</v>
       </c>
       <c r="N323" s="7" t="n">
         <f aca="false">M323-L323</f>
-        <v>15570.22</v>
+        <v>33325.53</v>
       </c>
       <c r="O323" s="5" t="n">
         <v>0</v>
@@ -42435,36 +42431,36 @@
         <v>0</v>
       </c>
       <c r="AE323" s="6" t="n">
-        <v>245.5</v>
+        <v>252.92</v>
       </c>
       <c r="AF323" s="7" t="n">
         <f aca="false">AE323-AD323</f>
-        <v>245.5</v>
+        <v>252.92</v>
       </c>
       <c r="AG323" s="5" t="n">
-        <v>12500</v>
+        <v>14622.58</v>
       </c>
       <c r="AH323" s="6" t="n">
-        <v>20553.35</v>
+        <v>47695.19</v>
       </c>
       <c r="AI323" s="7" t="n">
         <f aca="false">AH323-AG323</f>
-        <v>8053.35</v>
+        <v>33072.61</v>
       </c>
       <c r="AJ323" s="5" t="n">
         <v>0</v>
       </c>
       <c r="AK323" s="6" t="n">
-        <v>7271.37</v>
+        <v>0</v>
       </c>
       <c r="AL323" s="7" t="n">
         <f aca="false">AK323-AJ323</f>
-        <v>7271.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="3" t="n">
-        <v>3210</v>
+        <v>5210</v>
       </c>
       <c r="B324" s="4" t="s">
         <v>201</v>
@@ -42499,14 +42495,14 @@
         <v>0</v>
       </c>
       <c r="L324" s="5" t="n">
-        <v>23360.73</v>
+        <v>12500</v>
       </c>
       <c r="M324" s="6" t="n">
-        <v>33587.324</v>
+        <v>28070.22</v>
       </c>
       <c r="N324" s="7" t="n">
         <f aca="false">M324-L324</f>
-        <v>10226.594</v>
+        <v>15570.22</v>
       </c>
       <c r="O324" s="5" t="n">
         <v>0</v>
@@ -42562,42 +42558,42 @@
         <v>0</v>
       </c>
       <c r="AE324" s="6" t="n">
-        <v>660.354</v>
+        <v>245.5</v>
       </c>
       <c r="AF324" s="7" t="n">
         <f aca="false">AE324-AD324</f>
-        <v>660.354</v>
+        <v>245.5</v>
       </c>
       <c r="AG324" s="5" t="n">
-        <v>14560.73</v>
+        <v>12500</v>
       </c>
       <c r="AH324" s="6" t="n">
-        <v>15915.62</v>
+        <v>20553.35</v>
       </c>
       <c r="AI324" s="7" t="n">
         <f aca="false">AH324-AG324</f>
-        <v>1354.89</v>
+        <v>8053.35</v>
       </c>
       <c r="AJ324" s="5" t="n">
-        <v>8800</v>
+        <v>0</v>
       </c>
       <c r="AK324" s="6" t="n">
-        <v>17011.35</v>
+        <v>7271.37</v>
       </c>
       <c r="AL324" s="7" t="n">
         <f aca="false">AK324-AJ324</f>
-        <v>8211.35</v>
+        <v>7271.37</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="3" t="n">
-        <v>3422</v>
+        <v>3210</v>
       </c>
       <c r="B325" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C325" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D325" s="3" t="s">
         <v>176</v>
@@ -42626,14 +42622,14 @@
         <v>0</v>
       </c>
       <c r="L325" s="5" t="n">
-        <v>8089.37</v>
+        <v>23360.73</v>
       </c>
       <c r="M325" s="6" t="n">
-        <v>33596.389</v>
+        <v>33587.324</v>
       </c>
       <c r="N325" s="7" t="n">
         <f aca="false">M325-L325</f>
-        <v>25507.019</v>
+        <v>10226.594</v>
       </c>
       <c r="O325" s="5" t="n">
         <v>0</v>
@@ -42689,45 +42685,45 @@
         <v>0</v>
       </c>
       <c r="AE325" s="6" t="n">
-        <v>2.459</v>
+        <v>660.354</v>
       </c>
       <c r="AF325" s="7" t="n">
         <f aca="false">AE325-AD325</f>
-        <v>2.459</v>
+        <v>660.354</v>
       </c>
       <c r="AG325" s="5" t="n">
-        <v>8089.37</v>
+        <v>14560.73</v>
       </c>
       <c r="AH325" s="6" t="n">
-        <v>33593.93</v>
+        <v>15915.62</v>
       </c>
       <c r="AI325" s="7" t="n">
         <f aca="false">AH325-AG325</f>
-        <v>25504.56</v>
+        <v>1354.89</v>
       </c>
       <c r="AJ325" s="5" t="n">
-        <v>0</v>
+        <v>8800</v>
       </c>
       <c r="AK325" s="6" t="n">
-        <v>0</v>
+        <v>17011.35</v>
       </c>
       <c r="AL325" s="7" t="n">
         <f aca="false">AK325-AJ325</f>
-        <v>0</v>
+        <v>8211.35</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="3" t="n">
-        <v>225</v>
+        <v>3422</v>
       </c>
       <c r="B326" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D326" s="3" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="E326" s="3" t="s">
         <v>151</v>
@@ -42753,14 +42749,14 @@
         <v>0</v>
       </c>
       <c r="L326" s="5" t="n">
-        <v>0</v>
+        <v>8089.37</v>
       </c>
       <c r="M326" s="6" t="n">
-        <v>277.05</v>
+        <v>33596.389</v>
       </c>
       <c r="N326" s="7" t="n">
         <f aca="false">M326-L326</f>
-        <v>277.05</v>
+        <v>25507.019</v>
       </c>
       <c r="O326" s="5" t="n">
         <v>0</v>
@@ -42816,21 +42812,21 @@
         <v>0</v>
       </c>
       <c r="AE326" s="6" t="n">
-        <v>24.79</v>
+        <v>2.459</v>
       </c>
       <c r="AF326" s="7" t="n">
         <f aca="false">AE326-AD326</f>
-        <v>24.79</v>
+        <v>2.459</v>
       </c>
       <c r="AG326" s="5" t="n">
-        <v>0</v>
+        <v>8089.37</v>
       </c>
       <c r="AH326" s="6" t="n">
-        <v>252.26</v>
+        <v>33593.93</v>
       </c>
       <c r="AI326" s="7" t="n">
         <f aca="false">AH326-AG326</f>
-        <v>252.26</v>
+        <v>25504.56</v>
       </c>
       <c r="AJ326" s="5" t="n">
         <v>0</v>
@@ -42845,16 +42841,16 @@
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="3" t="n">
-        <v>2423</v>
+        <v>225</v>
       </c>
       <c r="B327" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C327" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D327" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E327" s="3" t="s">
         <v>151</v>
@@ -42880,14 +42876,14 @@
         <v>0</v>
       </c>
       <c r="L327" s="5" t="n">
-        <v>16666.7</v>
+        <v>0</v>
       </c>
       <c r="M327" s="6" t="n">
-        <v>18960.12</v>
+        <v>277.05</v>
       </c>
       <c r="N327" s="7" t="n">
         <f aca="false">M327-L327</f>
-        <v>2293.42</v>
+        <v>277.05</v>
       </c>
       <c r="O327" s="5" t="n">
         <v>0</v>
@@ -42943,21 +42939,21 @@
         <v>0</v>
       </c>
       <c r="AE327" s="6" t="n">
-        <v>0</v>
+        <v>24.79</v>
       </c>
       <c r="AF327" s="7" t="n">
         <f aca="false">AE327-AD327</f>
-        <v>0</v>
+        <v>24.79</v>
       </c>
       <c r="AG327" s="5" t="n">
-        <v>16666.7</v>
+        <v>0</v>
       </c>
       <c r="AH327" s="6" t="n">
-        <v>18960.12</v>
+        <v>252.26</v>
       </c>
       <c r="AI327" s="7" t="n">
         <f aca="false">AH327-AG327</f>
-        <v>2293.42</v>
+        <v>252.26</v>
       </c>
       <c r="AJ327" s="5" t="n">
         <v>0</v>
@@ -42972,10 +42968,10 @@
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="3" t="n">
-        <v>3223</v>
+        <v>2423</v>
       </c>
       <c r="B328" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>39</v>
@@ -43007,14 +43003,14 @@
         <v>0</v>
       </c>
       <c r="L328" s="5" t="n">
-        <v>50009.89</v>
+        <v>16666.7</v>
       </c>
       <c r="M328" s="6" t="n">
-        <v>59963.08</v>
+        <v>18960.12</v>
       </c>
       <c r="N328" s="7" t="n">
         <f aca="false">M328-L328</f>
-        <v>9953.19</v>
+        <v>2293.42</v>
       </c>
       <c r="O328" s="5" t="n">
         <v>0</v>
@@ -43077,14 +43073,14 @@
         <v>0</v>
       </c>
       <c r="AG328" s="5" t="n">
-        <v>50009.89</v>
+        <v>16666.7</v>
       </c>
       <c r="AH328" s="6" t="n">
-        <v>59963.08</v>
+        <v>18960.12</v>
       </c>
       <c r="AI328" s="7" t="n">
         <f aca="false">AH328-AG328</f>
-        <v>9953.19</v>
+        <v>2293.42</v>
       </c>
       <c r="AJ328" s="5" t="n">
         <v>0</v>
@@ -43099,13 +43095,13 @@
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="3" t="n">
-        <v>1820</v>
+        <v>3223</v>
       </c>
       <c r="B329" s="4" t="s">
         <v>205</v>
       </c>
       <c r="C329" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D329" s="3" t="s">
         <v>65</v>
@@ -43134,14 +43130,14 @@
         <v>0</v>
       </c>
       <c r="L329" s="5" t="n">
-        <v>50000</v>
+        <v>50009.89</v>
       </c>
       <c r="M329" s="6" t="n">
-        <v>0</v>
+        <v>59963.08</v>
       </c>
       <c r="N329" s="7" t="n">
         <f aca="false">M329-L329</f>
-        <v>-50000</v>
+        <v>9953.19</v>
       </c>
       <c r="O329" s="5" t="n">
         <v>0</v>
@@ -43204,14 +43200,14 @@
         <v>0</v>
       </c>
       <c r="AG329" s="5" t="n">
-        <v>50000</v>
+        <v>50009.89</v>
       </c>
       <c r="AH329" s="6" t="n">
-        <v>0</v>
+        <v>59963.08</v>
       </c>
       <c r="AI329" s="7" t="n">
         <f aca="false">AH329-AG329</f>
-        <v>-50000</v>
+        <v>9953.19</v>
       </c>
       <c r="AJ329" s="5" t="n">
         <v>0</v>
@@ -43226,7 +43222,7 @@
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="3" t="n">
-        <v>4423</v>
+        <v>1820</v>
       </c>
       <c r="B330" s="4" t="s">
         <v>205</v>
@@ -43261,14 +43257,14 @@
         <v>0</v>
       </c>
       <c r="L330" s="5" t="n">
-        <v>69999.99</v>
+        <v>50000</v>
       </c>
       <c r="M330" s="6" t="n">
-        <v>33806.19</v>
+        <v>0</v>
       </c>
       <c r="N330" s="7" t="n">
         <f aca="false">M330-L330</f>
-        <v>-36193.8</v>
+        <v>-50000</v>
       </c>
       <c r="O330" s="5" t="n">
         <v>0</v>
@@ -43331,14 +43327,14 @@
         <v>0</v>
       </c>
       <c r="AG330" s="5" t="n">
-        <v>69999.99</v>
+        <v>50000</v>
       </c>
       <c r="AH330" s="6" t="n">
-        <v>33806.19</v>
+        <v>0</v>
       </c>
       <c r="AI330" s="7" t="n">
         <f aca="false">AH330-AG330</f>
-        <v>-36193.8</v>
+        <v>-50000</v>
       </c>
       <c r="AJ330" s="5" t="n">
         <v>0</v>
@@ -43353,13 +43349,13 @@
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="3" t="n">
-        <v>5223</v>
+        <v>4423</v>
       </c>
       <c r="B331" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C331" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D331" s="3" t="s">
         <v>65</v>
@@ -43388,14 +43384,14 @@
         <v>0</v>
       </c>
       <c r="L331" s="5" t="n">
-        <v>9911.85</v>
+        <v>69999.99</v>
       </c>
       <c r="M331" s="6" t="n">
-        <v>6764</v>
+        <v>33806.19</v>
       </c>
       <c r="N331" s="7" t="n">
         <f aca="false">M331-L331</f>
-        <v>-3147.85</v>
+        <v>-36193.8</v>
       </c>
       <c r="O331" s="5" t="n">
         <v>0</v>
@@ -43458,14 +43454,14 @@
         <v>0</v>
       </c>
       <c r="AG331" s="5" t="n">
-        <v>9911.85</v>
+        <v>69999.99</v>
       </c>
       <c r="AH331" s="6" t="n">
-        <v>6764</v>
+        <v>33806.19</v>
       </c>
       <c r="AI331" s="7" t="n">
         <f aca="false">AH331-AG331</f>
-        <v>-3147.85</v>
+        <v>-36193.8</v>
       </c>
       <c r="AJ331" s="5" t="n">
         <v>0</v>
@@ -43480,16 +43476,16 @@
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="3" t="n">
-        <v>6417</v>
+        <v>5223</v>
       </c>
       <c r="B332" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C332" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D332" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E332" s="3" t="s">
         <v>151</v>
@@ -43515,14 +43511,14 @@
         <v>0</v>
       </c>
       <c r="L332" s="5" t="n">
-        <v>0</v>
+        <v>9911.85</v>
       </c>
       <c r="M332" s="6" t="n">
-        <v>0</v>
+        <v>6764</v>
       </c>
       <c r="N332" s="7" t="n">
         <f aca="false">M332-L332</f>
-        <v>0</v>
+        <v>-3147.85</v>
       </c>
       <c r="O332" s="5" t="n">
         <v>0</v>
@@ -43585,14 +43581,14 @@
         <v>0</v>
       </c>
       <c r="AG332" s="5" t="n">
-        <v>0</v>
+        <v>9911.85</v>
       </c>
       <c r="AH332" s="6" t="n">
-        <v>0</v>
+        <v>6764</v>
       </c>
       <c r="AI332" s="7" t="n">
         <f aca="false">AH332-AG332</f>
-        <v>0</v>
+        <v>-3147.85</v>
       </c>
       <c r="AJ332" s="5" t="n">
         <v>0</v>
@@ -43607,13 +43603,13 @@
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="3" t="n">
-        <v>6223</v>
+        <v>6417</v>
       </c>
       <c r="B333" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C333" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D333" s="3" t="s">
         <v>55</v>
@@ -43642,14 +43638,14 @@
         <v>0</v>
       </c>
       <c r="L333" s="5" t="n">
-        <v>18277.55</v>
+        <v>0</v>
       </c>
       <c r="M333" s="6" t="n">
-        <v>14110.347</v>
+        <v>0</v>
       </c>
       <c r="N333" s="7" t="n">
         <f aca="false">M333-L333</f>
-        <v>-4167.203</v>
+        <v>0</v>
       </c>
       <c r="O333" s="5" t="n">
         <v>0</v>
@@ -43705,21 +43701,21 @@
         <v>0</v>
       </c>
       <c r="AE333" s="6" t="n">
-        <v>185.227</v>
+        <v>0</v>
       </c>
       <c r="AF333" s="7" t="n">
         <f aca="false">AE333-AD333</f>
-        <v>185.227</v>
+        <v>0</v>
       </c>
       <c r="AG333" s="5" t="n">
-        <v>18277.55</v>
+        <v>0</v>
       </c>
       <c r="AH333" s="6" t="n">
-        <v>13925.12</v>
+        <v>0</v>
       </c>
       <c r="AI333" s="7" t="n">
         <f aca="false">AH333-AG333</f>
-        <v>-4352.43</v>
+        <v>0</v>
       </c>
       <c r="AJ333" s="5" t="n">
         <v>0</v>
@@ -43734,13 +43730,13 @@
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="3" t="n">
-        <v>9221</v>
+        <v>6223</v>
       </c>
       <c r="B334" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C334" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D334" s="3" t="s">
         <v>55</v>
@@ -43769,14 +43765,14 @@
         <v>0</v>
       </c>
       <c r="L334" s="5" t="n">
-        <v>0</v>
+        <v>18277.55</v>
       </c>
       <c r="M334" s="6" t="n">
-        <v>1652.91</v>
+        <v>14110.347</v>
       </c>
       <c r="N334" s="7" t="n">
         <f aca="false">M334-L334</f>
-        <v>1652.91</v>
+        <v>-4167.203</v>
       </c>
       <c r="O334" s="5" t="n">
         <v>0</v>
@@ -43832,21 +43828,21 @@
         <v>0</v>
       </c>
       <c r="AE334" s="6" t="n">
-        <v>0</v>
+        <v>185.227</v>
       </c>
       <c r="AF334" s="7" t="n">
         <f aca="false">AE334-AD334</f>
-        <v>0</v>
+        <v>185.227</v>
       </c>
       <c r="AG334" s="5" t="n">
-        <v>0</v>
+        <v>18277.55</v>
       </c>
       <c r="AH334" s="6" t="n">
-        <v>1652.91</v>
+        <v>13925.12</v>
       </c>
       <c r="AI334" s="7" t="n">
         <f aca="false">AH334-AG334</f>
-        <v>1652.91</v>
+        <v>-4352.43</v>
       </c>
       <c r="AJ334" s="5" t="n">
         <v>0</v>
@@ -43861,13 +43857,13 @@
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="3" t="n">
-        <v>8214</v>
+        <v>9221</v>
       </c>
       <c r="B335" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C335" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D335" s="3" t="s">
         <v>55</v>
@@ -43896,14 +43892,14 @@
         <v>0</v>
       </c>
       <c r="L335" s="5" t="n">
-        <v>493256.35</v>
+        <v>0</v>
       </c>
       <c r="M335" s="6" t="n">
-        <v>627093.33</v>
+        <v>1652.91</v>
       </c>
       <c r="N335" s="7" t="n">
         <f aca="false">M335-L335</f>
-        <v>133836.98</v>
+        <v>1652.91</v>
       </c>
       <c r="O335" s="5" t="n">
         <v>0</v>
@@ -43939,11 +43935,11 @@
         <v>0</v>
       </c>
       <c r="Y335" s="6" t="n">
-        <v>1498.6</v>
+        <v>0</v>
       </c>
       <c r="Z335" s="7" t="n">
         <f aca="false">Y335-X335</f>
-        <v>1498.6</v>
+        <v>0</v>
       </c>
       <c r="AA335" s="5" t="n">
         <v>0</v>
@@ -43959,36 +43955,36 @@
         <v>0</v>
       </c>
       <c r="AE335" s="6" t="n">
-        <v>6926.44</v>
+        <v>0</v>
       </c>
       <c r="AF335" s="7" t="n">
         <f aca="false">AE335-AD335</f>
-        <v>6926.44</v>
+        <v>0</v>
       </c>
       <c r="AG335" s="5" t="n">
-        <v>493256.35</v>
+        <v>0</v>
       </c>
       <c r="AH335" s="6" t="n">
-        <v>547044.66</v>
+        <v>1652.91</v>
       </c>
       <c r="AI335" s="7" t="n">
         <f aca="false">AH335-AG335</f>
-        <v>53788.3100000001</v>
+        <v>1652.91</v>
       </c>
       <c r="AJ335" s="5" t="n">
         <v>0</v>
       </c>
       <c r="AK335" s="6" t="n">
-        <v>71623.63</v>
+        <v>0</v>
       </c>
       <c r="AL335" s="7" t="n">
         <f aca="false">AK335-AJ335</f>
-        <v>71623.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="3" t="n">
-        <v>9214</v>
+        <v>8214</v>
       </c>
       <c r="B336" s="4" t="s">
         <v>210</v>
@@ -44023,14 +44019,14 @@
         <v>0</v>
       </c>
       <c r="L336" s="5" t="n">
-        <v>480106.05</v>
+        <v>493256.35</v>
       </c>
       <c r="M336" s="6" t="n">
-        <v>621009.882</v>
+        <v>627093.33</v>
       </c>
       <c r="N336" s="7" t="n">
         <f aca="false">M336-L336</f>
-        <v>140903.832</v>
+        <v>133836.98</v>
       </c>
       <c r="O336" s="5" t="n">
         <v>0</v>
@@ -44066,11 +44062,11 @@
         <v>0</v>
       </c>
       <c r="Y336" s="6" t="n">
-        <v>1388.4</v>
+        <v>1498.6</v>
       </c>
       <c r="Z336" s="7" t="n">
         <f aca="false">Y336-X336</f>
-        <v>1388.4</v>
+        <v>1498.6</v>
       </c>
       <c r="AA336" s="5" t="n">
         <v>0</v>
@@ -44086,42 +44082,42 @@
         <v>0</v>
       </c>
       <c r="AE336" s="6" t="n">
-        <v>9409.572</v>
+        <v>6926.44</v>
       </c>
       <c r="AF336" s="7" t="n">
         <f aca="false">AE336-AD336</f>
-        <v>9409.572</v>
+        <v>6926.44</v>
       </c>
       <c r="AG336" s="5" t="n">
-        <v>480106.05</v>
+        <v>493256.35</v>
       </c>
       <c r="AH336" s="6" t="n">
-        <v>610211.91</v>
+        <v>547044.66</v>
       </c>
       <c r="AI336" s="7" t="n">
         <f aca="false">AH336-AG336</f>
-        <v>130105.86</v>
+        <v>53788.3100000001</v>
       </c>
       <c r="AJ336" s="5" t="n">
         <v>0</v>
       </c>
       <c r="AK336" s="6" t="n">
-        <v>0</v>
+        <v>71623.63</v>
       </c>
       <c r="AL336" s="7" t="n">
         <f aca="false">AK336-AJ336</f>
-        <v>0</v>
+        <v>71623.63</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="3" t="n">
-        <v>92</v>
+        <v>9214</v>
       </c>
       <c r="B337" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C337" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D337" s="3" t="s">
         <v>55</v>
@@ -44150,14 +44146,14 @@
         <v>0</v>
       </c>
       <c r="L337" s="5" t="n">
-        <v>8819</v>
+        <v>480106.05</v>
       </c>
       <c r="M337" s="6" t="n">
-        <v>3863.74</v>
+        <v>621009.882</v>
       </c>
       <c r="N337" s="7" t="n">
         <f aca="false">M337-L337</f>
-        <v>-4955.26</v>
+        <v>140903.832</v>
       </c>
       <c r="O337" s="5" t="n">
         <v>0</v>
@@ -44193,11 +44189,11 @@
         <v>0</v>
       </c>
       <c r="Y337" s="6" t="n">
-        <v>0</v>
+        <v>1388.4</v>
       </c>
       <c r="Z337" s="7" t="n">
         <f aca="false">Y337-X337</f>
-        <v>0</v>
+        <v>1388.4</v>
       </c>
       <c r="AA337" s="5" t="n">
         <v>0</v>
@@ -44213,21 +44209,21 @@
         <v>0</v>
       </c>
       <c r="AE337" s="6" t="n">
-        <v>0</v>
+        <v>9409.572</v>
       </c>
       <c r="AF337" s="7" t="n">
         <f aca="false">AE337-AD337</f>
-        <v>0</v>
+        <v>9409.572</v>
       </c>
       <c r="AG337" s="5" t="n">
-        <v>8819</v>
+        <v>480106.05</v>
       </c>
       <c r="AH337" s="6" t="n">
-        <v>3863.74</v>
+        <v>610211.91</v>
       </c>
       <c r="AI337" s="7" t="n">
         <f aca="false">AH337-AG337</f>
-        <v>-4955.26</v>
+        <v>130105.86</v>
       </c>
       <c r="AJ337" s="5" t="n">
         <v>0</v>
@@ -44242,13 +44238,13 @@
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="3" t="n">
-        <v>10422</v>
+        <v>92</v>
       </c>
       <c r="B338" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C338" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D338" s="3" t="s">
         <v>55</v>
@@ -44277,14 +44273,14 @@
         <v>0</v>
       </c>
       <c r="L338" s="5" t="n">
-        <v>49693</v>
+        <v>8819</v>
       </c>
       <c r="M338" s="6" t="n">
-        <v>10252.455</v>
+        <v>3863.74</v>
       </c>
       <c r="N338" s="7" t="n">
         <f aca="false">M338-L338</f>
-        <v>-39440.545</v>
+        <v>-4955.26</v>
       </c>
       <c r="O338" s="5" t="n">
         <v>0</v>
@@ -44340,42 +44336,42 @@
         <v>0</v>
       </c>
       <c r="AE338" s="6" t="n">
-        <v>235.655</v>
+        <v>0</v>
       </c>
       <c r="AF338" s="7" t="n">
         <f aca="false">AE338-AD338</f>
-        <v>235.655</v>
+        <v>0</v>
       </c>
       <c r="AG338" s="5" t="n">
-        <v>46693</v>
+        <v>8819</v>
       </c>
       <c r="AH338" s="6" t="n">
-        <v>10016.8</v>
+        <v>3863.74</v>
       </c>
       <c r="AI338" s="7" t="n">
         <f aca="false">AH338-AG338</f>
-        <v>-36676.2</v>
+        <v>-4955.26</v>
       </c>
       <c r="AJ338" s="5" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AK338" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL338" s="7" t="n">
         <f aca="false">AK338-AJ338</f>
-        <v>-3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="3" t="n">
-        <v>2817</v>
+        <v>10422</v>
       </c>
       <c r="B339" s="4" t="s">
         <v>212</v>
       </c>
       <c r="C339" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D339" s="3" t="s">
         <v>55</v>
@@ -44404,14 +44400,14 @@
         <v>0</v>
       </c>
       <c r="L339" s="5" t="n">
-        <v>0</v>
+        <v>49693</v>
       </c>
       <c r="M339" s="6" t="n">
-        <v>0</v>
+        <v>10252.455</v>
       </c>
       <c r="N339" s="7" t="n">
         <f aca="false">M339-L339</f>
-        <v>0</v>
+        <v>-39440.545</v>
       </c>
       <c r="O339" s="5" t="n">
         <v>0</v>
@@ -44467,42 +44463,42 @@
         <v>0</v>
       </c>
       <c r="AE339" s="6" t="n">
-        <v>0</v>
+        <v>235.655</v>
       </c>
       <c r="AF339" s="7" t="n">
         <f aca="false">AE339-AD339</f>
-        <v>0</v>
+        <v>235.655</v>
       </c>
       <c r="AG339" s="5" t="n">
-        <v>0</v>
+        <v>46693</v>
       </c>
       <c r="AH339" s="6" t="n">
-        <v>0</v>
+        <v>10016.8</v>
       </c>
       <c r="AI339" s="7" t="n">
         <f aca="false">AH339-AG339</f>
-        <v>0</v>
+        <v>-36676.2</v>
       </c>
       <c r="AJ339" s="5" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="AK339" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL339" s="7" t="n">
         <f aca="false">AK339-AJ339</f>
-        <v>0</v>
+        <v>-3000</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="3" t="n">
-        <v>3615</v>
+        <v>2817</v>
       </c>
       <c r="B340" s="4" t="s">
         <v>212</v>
       </c>
       <c r="C340" s="3" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="D340" s="3" t="s">
         <v>55</v>
@@ -44531,14 +44527,14 @@
         <v>0</v>
       </c>
       <c r="L340" s="5" t="n">
-        <v>18181.81</v>
+        <v>0</v>
       </c>
       <c r="M340" s="6" t="n">
-        <v>1582.028</v>
+        <v>0</v>
       </c>
       <c r="N340" s="7" t="n">
         <f aca="false">M340-L340</f>
-        <v>-16599.782</v>
+        <v>0</v>
       </c>
       <c r="O340" s="5" t="n">
         <v>0</v>
@@ -44594,42 +44590,42 @@
         <v>0</v>
       </c>
       <c r="AE340" s="6" t="n">
-        <v>11.908</v>
+        <v>0</v>
       </c>
       <c r="AF340" s="7" t="n">
         <f aca="false">AE340-AD340</f>
-        <v>11.908</v>
+        <v>0</v>
       </c>
       <c r="AG340" s="5" t="n">
-        <v>8181.81</v>
+        <v>0</v>
       </c>
       <c r="AH340" s="6" t="n">
-        <v>1570.12</v>
+        <v>0</v>
       </c>
       <c r="AI340" s="7" t="n">
         <f aca="false">AH340-AG340</f>
-        <v>-6611.69</v>
+        <v>0</v>
       </c>
       <c r="AJ340" s="5" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="AK340" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL340" s="7" t="n">
         <f aca="false">AK340-AJ340</f>
-        <v>-10000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="3" t="n">
-        <v>2215</v>
+        <v>3615</v>
       </c>
       <c r="B341" s="4" t="s">
         <v>212</v>
       </c>
       <c r="C341" s="3" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D341" s="3" t="s">
         <v>55</v>
@@ -44658,14 +44654,14 @@
         <v>0</v>
       </c>
       <c r="L341" s="5" t="n">
-        <v>94291.49</v>
+        <v>18181.81</v>
       </c>
       <c r="M341" s="6" t="n">
-        <v>63017.115</v>
+        <v>1582.028</v>
       </c>
       <c r="N341" s="7" t="n">
         <f aca="false">M341-L341</f>
-        <v>-31274.375</v>
+        <v>-16599.782</v>
       </c>
       <c r="O341" s="5" t="n">
         <v>0</v>
@@ -44721,42 +44717,42 @@
         <v>0</v>
       </c>
       <c r="AE341" s="6" t="n">
-        <v>131.235</v>
+        <v>11.908</v>
       </c>
       <c r="AF341" s="7" t="n">
         <f aca="false">AE341-AD341</f>
-        <v>131.235</v>
+        <v>11.908</v>
       </c>
       <c r="AG341" s="5" t="n">
-        <v>64291.49</v>
+        <v>8181.81</v>
       </c>
       <c r="AH341" s="6" t="n">
-        <v>62885.88</v>
+        <v>1570.12</v>
       </c>
       <c r="AI341" s="7" t="n">
         <f aca="false">AH341-AG341</f>
-        <v>-1405.61</v>
+        <v>-6611.69</v>
       </c>
       <c r="AJ341" s="5" t="n">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="AK341" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL341" s="7" t="n">
         <f aca="false">AK341-AJ341</f>
-        <v>-30000</v>
+        <v>-10000</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="3" t="n">
-        <v>1417</v>
+        <v>2215</v>
       </c>
       <c r="B342" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C342" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D342" s="3" t="s">
         <v>55</v>
@@ -44785,14 +44781,14 @@
         <v>0</v>
       </c>
       <c r="L342" s="5" t="n">
-        <v>8454.57</v>
+        <v>94291.49</v>
       </c>
       <c r="M342" s="6" t="n">
-        <v>15.576</v>
+        <v>63017.115</v>
       </c>
       <c r="N342" s="7" t="n">
         <f aca="false">M342-L342</f>
-        <v>-8438.994</v>
+        <v>-31274.375</v>
       </c>
       <c r="O342" s="5" t="n">
         <v>0</v>
@@ -44848,39 +44844,39 @@
         <v>0</v>
       </c>
       <c r="AE342" s="6" t="n">
-        <v>10.476</v>
+        <v>131.235</v>
       </c>
       <c r="AF342" s="7" t="n">
         <f aca="false">AE342-AD342</f>
-        <v>10.476</v>
+        <v>131.235</v>
       </c>
       <c r="AG342" s="5" t="n">
-        <v>2454.57</v>
+        <v>64291.49</v>
       </c>
       <c r="AH342" s="6" t="n">
-        <v>5.1</v>
+        <v>62885.88</v>
       </c>
       <c r="AI342" s="7" t="n">
         <f aca="false">AH342-AG342</f>
-        <v>-2449.47</v>
+        <v>-1405.61</v>
       </c>
       <c r="AJ342" s="5" t="n">
-        <v>6000</v>
+        <v>30000</v>
       </c>
       <c r="AK342" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL342" s="7" t="n">
         <f aca="false">AK342-AJ342</f>
-        <v>-6000</v>
+        <v>-30000</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="3" t="n">
-        <v>7223</v>
+        <v>1417</v>
       </c>
       <c r="B343" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C343" s="3" t="s">
         <v>52</v>
@@ -44912,14 +44908,14 @@
         <v>0</v>
       </c>
       <c r="L343" s="5" t="n">
-        <v>66666.7</v>
+        <v>8454.57</v>
       </c>
       <c r="M343" s="6" t="n">
-        <v>1662.14</v>
+        <v>15.576</v>
       </c>
       <c r="N343" s="7" t="n">
         <f aca="false">M343-L343</f>
-        <v>-65004.56</v>
+        <v>-8438.994</v>
       </c>
       <c r="O343" s="5" t="n">
         <v>0</v>
@@ -44975,42 +44971,42 @@
         <v>0</v>
       </c>
       <c r="AE343" s="6" t="n">
-        <v>0</v>
+        <v>10.476</v>
       </c>
       <c r="AF343" s="7" t="n">
         <f aca="false">AE343-AD343</f>
-        <v>0</v>
+        <v>10.476</v>
       </c>
       <c r="AG343" s="5" t="n">
-        <v>66666.7</v>
+        <v>2454.57</v>
       </c>
       <c r="AH343" s="6" t="n">
-        <v>1662.14</v>
+        <v>5.1</v>
       </c>
       <c r="AI343" s="7" t="n">
         <f aca="false">AH343-AG343</f>
-        <v>-65004.56</v>
+        <v>-2449.47</v>
       </c>
       <c r="AJ343" s="5" t="n">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="AK343" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL343" s="7" t="n">
         <f aca="false">AK343-AJ343</f>
-        <v>0</v>
+        <v>-6000</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="3" t="n">
-        <v>4222</v>
+        <v>7223</v>
       </c>
       <c r="B344" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C344" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D344" s="3" t="s">
         <v>55</v>
@@ -45039,14 +45035,14 @@
         <v>0</v>
       </c>
       <c r="L344" s="5" t="n">
-        <v>12637.28</v>
+        <v>66666.7</v>
       </c>
       <c r="M344" s="6" t="n">
-        <v>10008.18</v>
+        <v>1662.14</v>
       </c>
       <c r="N344" s="7" t="n">
         <f aca="false">M344-L344</f>
-        <v>-2629.1</v>
+        <v>-65004.56</v>
       </c>
       <c r="O344" s="5" t="n">
         <v>0</v>
@@ -45109,14 +45105,14 @@
         <v>0</v>
       </c>
       <c r="AG344" s="5" t="n">
-        <v>12637.28</v>
+        <v>66666.7</v>
       </c>
       <c r="AH344" s="6" t="n">
-        <v>10008.18</v>
+        <v>1662.14</v>
       </c>
       <c r="AI344" s="7" t="n">
         <f aca="false">AH344-AG344</f>
-        <v>-2629.1</v>
+        <v>-65004.56</v>
       </c>
       <c r="AJ344" s="5" t="n">
         <v>0</v>
@@ -45131,13 +45127,13 @@
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="3" t="n">
-        <v>1817</v>
+        <v>4222</v>
       </c>
       <c r="B345" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C345" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D345" s="3" t="s">
         <v>55</v>
@@ -45166,14 +45162,14 @@
         <v>0</v>
       </c>
       <c r="L345" s="5" t="n">
-        <v>167070.98</v>
+        <v>12637.28</v>
       </c>
       <c r="M345" s="6" t="n">
-        <v>144371.094</v>
+        <v>10008.18</v>
       </c>
       <c r="N345" s="7" t="n">
         <f aca="false">M345-L345</f>
-        <v>-22699.886</v>
+        <v>-2629.1</v>
       </c>
       <c r="O345" s="5" t="n">
         <v>0</v>
@@ -45209,11 +45205,11 @@
         <v>0</v>
       </c>
       <c r="Y345" s="6" t="n">
-        <v>2063.25</v>
+        <v>0</v>
       </c>
       <c r="Z345" s="7" t="n">
         <f aca="false">Y345-X345</f>
-        <v>2063.25</v>
+        <v>0</v>
       </c>
       <c r="AA345" s="5" t="n">
         <v>0</v>
@@ -45229,42 +45225,42 @@
         <v>0</v>
       </c>
       <c r="AE345" s="6" t="n">
-        <v>345.064</v>
+        <v>0</v>
       </c>
       <c r="AF345" s="7" t="n">
         <f aca="false">AE345-AD345</f>
-        <v>345.064</v>
+        <v>0</v>
       </c>
       <c r="AG345" s="5" t="n">
-        <v>47070.98</v>
+        <v>12637.28</v>
       </c>
       <c r="AH345" s="6" t="n">
-        <v>56736.1</v>
+        <v>10008.18</v>
       </c>
       <c r="AI345" s="7" t="n">
         <f aca="false">AH345-AG345</f>
-        <v>9665.12</v>
+        <v>-2629.1</v>
       </c>
       <c r="AJ345" s="5" t="n">
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="AK345" s="6" t="n">
-        <v>85226.68</v>
+        <v>0</v>
       </c>
       <c r="AL345" s="7" t="n">
         <f aca="false">AK345-AJ345</f>
-        <v>-34773.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="3" t="n">
-        <v>9418</v>
+        <v>1817</v>
       </c>
       <c r="B346" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C346" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D346" s="3" t="s">
         <v>55</v>
@@ -45293,14 +45289,14 @@
         <v>0</v>
       </c>
       <c r="L346" s="5" t="n">
-        <v>100449.2</v>
+        <v>167070.98</v>
       </c>
       <c r="M346" s="6" t="n">
-        <v>223633.9526</v>
+        <v>144371.094</v>
       </c>
       <c r="N346" s="7" t="n">
         <f aca="false">M346-L346</f>
-        <v>123184.7526</v>
+        <v>-22699.886</v>
       </c>
       <c r="O346" s="5" t="n">
         <v>0</v>
@@ -45336,11 +45332,11 @@
         <v>0</v>
       </c>
       <c r="Y346" s="6" t="n">
-        <v>9037.72</v>
+        <v>2063.25</v>
       </c>
       <c r="Z346" s="7" t="n">
         <f aca="false">Y346-X346</f>
-        <v>9037.72</v>
+        <v>2063.25</v>
       </c>
       <c r="AA346" s="5" t="n">
         <v>0</v>
@@ -45356,42 +45352,42 @@
         <v>0</v>
       </c>
       <c r="AE346" s="6" t="n">
-        <v>1121.2626</v>
+        <v>345.064</v>
       </c>
       <c r="AF346" s="7" t="n">
         <f aca="false">AE346-AD346</f>
-        <v>1121.2626</v>
+        <v>345.064</v>
       </c>
       <c r="AG346" s="5" t="n">
-        <v>100449.2</v>
+        <v>47070.98</v>
       </c>
       <c r="AH346" s="6" t="n">
-        <v>213474.97</v>
+        <v>56736.1</v>
       </c>
       <c r="AI346" s="7" t="n">
         <f aca="false">AH346-AG346</f>
-        <v>113025.77</v>
+        <v>9665.12</v>
       </c>
       <c r="AJ346" s="5" t="n">
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="AK346" s="6" t="n">
-        <v>0</v>
+        <v>85226.68</v>
       </c>
       <c r="AL346" s="7" t="n">
         <f aca="false">AK346-AJ346</f>
-        <v>0</v>
+        <v>-34773.32</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="3" t="n">
-        <v>7010</v>
+        <v>9418</v>
       </c>
       <c r="B347" s="4" t="s">
         <v>217</v>
       </c>
       <c r="C347" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D347" s="3" t="s">
         <v>55</v>
@@ -45420,14 +45416,14 @@
         <v>0</v>
       </c>
       <c r="L347" s="5" t="n">
-        <v>0</v>
+        <v>100449.2</v>
       </c>
       <c r="M347" s="6" t="n">
-        <v>0</v>
+        <v>223633.9526</v>
       </c>
       <c r="N347" s="7" t="n">
         <f aca="false">M347-L347</f>
-        <v>0</v>
+        <v>123184.7526</v>
       </c>
       <c r="O347" s="5" t="n">
         <v>0</v>
@@ -45463,11 +45459,11 @@
         <v>0</v>
       </c>
       <c r="Y347" s="6" t="n">
-        <v>0</v>
+        <v>9037.72</v>
       </c>
       <c r="Z347" s="7" t="n">
         <f aca="false">Y347-X347</f>
-        <v>0</v>
+        <v>9037.72</v>
       </c>
       <c r="AA347" s="5" t="n">
         <v>0</v>
@@ -45483,21 +45479,21 @@
         <v>0</v>
       </c>
       <c r="AE347" s="6" t="n">
-        <v>0</v>
+        <v>1121.2626</v>
       </c>
       <c r="AF347" s="7" t="n">
         <f aca="false">AE347-AD347</f>
-        <v>0</v>
+        <v>1121.2626</v>
       </c>
       <c r="AG347" s="5" t="n">
-        <v>0</v>
+        <v>100449.2</v>
       </c>
       <c r="AH347" s="6" t="n">
-        <v>0</v>
+        <v>213474.97</v>
       </c>
       <c r="AI347" s="7" t="n">
         <f aca="false">AH347-AG347</f>
-        <v>0</v>
+        <v>113025.77</v>
       </c>
       <c r="AJ347" s="5" t="n">
         <v>0</v>
@@ -45512,13 +45508,13 @@
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="3" t="n">
-        <v>415</v>
+        <v>7010</v>
       </c>
       <c r="B348" s="4" t="s">
         <v>217</v>
       </c>
       <c r="C348" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D348" s="3" t="s">
         <v>55</v>
@@ -45547,14 +45543,14 @@
         <v>0</v>
       </c>
       <c r="L348" s="5" t="n">
-        <v>66394.63</v>
+        <v>0</v>
       </c>
       <c r="M348" s="6" t="n">
-        <v>11207.046</v>
+        <v>0</v>
       </c>
       <c r="N348" s="7" t="n">
         <f aca="false">M348-L348</f>
-        <v>-55187.584</v>
+        <v>0</v>
       </c>
       <c r="O348" s="5" t="n">
         <v>0</v>
@@ -45590,11 +45586,11 @@
         <v>0</v>
       </c>
       <c r="Y348" s="6" t="n">
-        <v>1564.384</v>
+        <v>0</v>
       </c>
       <c r="Z348" s="7" t="n">
         <f aca="false">Y348-X348</f>
-        <v>1564.384</v>
+        <v>0</v>
       </c>
       <c r="AA348" s="5" t="n">
         <v>0</v>
@@ -45610,39 +45606,39 @@
         <v>0</v>
       </c>
       <c r="AE348" s="6" t="n">
-        <v>138.942</v>
+        <v>0</v>
       </c>
       <c r="AF348" s="7" t="n">
         <f aca="false">AE348-AD348</f>
-        <v>138.942</v>
+        <v>0</v>
       </c>
       <c r="AG348" s="5" t="n">
-        <v>16394.63</v>
+        <v>0</v>
       </c>
       <c r="AH348" s="6" t="n">
-        <v>9503.72</v>
+        <v>0</v>
       </c>
       <c r="AI348" s="7" t="n">
         <f aca="false">AH348-AG348</f>
-        <v>-6890.91</v>
+        <v>0</v>
       </c>
       <c r="AJ348" s="5" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="AK348" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL348" s="7" t="n">
         <f aca="false">AK348-AJ348</f>
-        <v>-50000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="3" t="n">
-        <v>2417</v>
+        <v>415</v>
       </c>
       <c r="B349" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>52</v>
@@ -45674,14 +45670,14 @@
         <v>0</v>
       </c>
       <c r="L349" s="5" t="n">
-        <v>6272.76</v>
+        <v>66394.63</v>
       </c>
       <c r="M349" s="6" t="n">
-        <v>2686.672</v>
+        <v>11207.046</v>
       </c>
       <c r="N349" s="7" t="n">
         <f aca="false">M349-L349</f>
-        <v>-3586.088</v>
+        <v>-55187.584</v>
       </c>
       <c r="O349" s="5" t="n">
         <v>0</v>
@@ -45717,11 +45713,11 @@
         <v>0</v>
       </c>
       <c r="Y349" s="6" t="n">
-        <v>145.75</v>
+        <v>1564.384</v>
       </c>
       <c r="Z349" s="7" t="n">
         <f aca="false">Y349-X349</f>
-        <v>145.75</v>
+        <v>1564.384</v>
       </c>
       <c r="AA349" s="5" t="n">
         <v>0</v>
@@ -45737,39 +45733,39 @@
         <v>0</v>
       </c>
       <c r="AE349" s="6" t="n">
-        <v>6.702</v>
+        <v>138.942</v>
       </c>
       <c r="AF349" s="7" t="n">
         <f aca="false">AE349-AD349</f>
-        <v>6.702</v>
+        <v>138.942</v>
       </c>
       <c r="AG349" s="5" t="n">
-        <v>3272.76</v>
+        <v>16394.63</v>
       </c>
       <c r="AH349" s="6" t="n">
-        <v>2534.22</v>
+        <v>9503.72</v>
       </c>
       <c r="AI349" s="7" t="n">
         <f aca="false">AH349-AG349</f>
-        <v>-738.54</v>
+        <v>-6890.91</v>
       </c>
       <c r="AJ349" s="5" t="n">
-        <v>3000</v>
+        <v>50000</v>
       </c>
       <c r="AK349" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL349" s="7" t="n">
         <f aca="false">AK349-AJ349</f>
-        <v>-3000</v>
+        <v>-50000</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="3" t="n">
-        <v>5415</v>
+        <v>2417</v>
       </c>
       <c r="B350" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C350" s="3" t="s">
         <v>52</v>
@@ -45801,14 +45797,14 @@
         <v>0</v>
       </c>
       <c r="L350" s="5" t="n">
-        <v>16666.7</v>
+        <v>6272.76</v>
       </c>
       <c r="M350" s="6" t="n">
-        <v>0</v>
+        <v>2686.672</v>
       </c>
       <c r="N350" s="7" t="n">
         <f aca="false">M350-L350</f>
-        <v>-16666.7</v>
+        <v>-3586.088</v>
       </c>
       <c r="O350" s="5" t="n">
         <v>0</v>
@@ -45844,11 +45840,11 @@
         <v>0</v>
       </c>
       <c r="Y350" s="6" t="n">
-        <v>0</v>
+        <v>145.75</v>
       </c>
       <c r="Z350" s="7" t="n">
         <f aca="false">Y350-X350</f>
-        <v>0</v>
+        <v>145.75</v>
       </c>
       <c r="AA350" s="5" t="n">
         <v>0</v>
@@ -45864,45 +45860,45 @@
         <v>0</v>
       </c>
       <c r="AE350" s="6" t="n">
-        <v>0</v>
+        <v>6.702</v>
       </c>
       <c r="AF350" s="7" t="n">
         <f aca="false">AE350-AD350</f>
-        <v>0</v>
+        <v>6.702</v>
       </c>
       <c r="AG350" s="5" t="n">
-        <v>16666.7</v>
+        <v>3272.76</v>
       </c>
       <c r="AH350" s="6" t="n">
-        <v>0</v>
+        <v>2534.22</v>
       </c>
       <c r="AI350" s="7" t="n">
         <f aca="false">AH350-AG350</f>
-        <v>-16666.7</v>
+        <v>-738.54</v>
       </c>
       <c r="AJ350" s="5" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="AK350" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL350" s="7" t="n">
         <f aca="false">AK350-AJ350</f>
-        <v>0</v>
+        <v>-3000</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="3" t="n">
-        <v>2315</v>
+        <v>5415</v>
       </c>
       <c r="B351" s="4" t="s">
-        <v>82</v>
+        <v>219</v>
       </c>
       <c r="C351" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D351" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E351" s="3" t="s">
         <v>151</v>
@@ -45928,14 +45924,14 @@
         <v>0</v>
       </c>
       <c r="L351" s="5" t="n">
-        <v>0</v>
+        <v>16666.7</v>
       </c>
       <c r="M351" s="6" t="n">
         <v>0</v>
       </c>
       <c r="N351" s="7" t="n">
         <f aca="false">M351-L351</f>
-        <v>0</v>
+        <v>-16666.7</v>
       </c>
       <c r="O351" s="5" t="n">
         <v>0</v>
@@ -45998,14 +45994,14 @@
         <v>0</v>
       </c>
       <c r="AG351" s="5" t="n">
-        <v>0</v>
+        <v>16666.7</v>
       </c>
       <c r="AH351" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AI351" s="7" t="n">
         <f aca="false">AH351-AG351</f>
-        <v>0</v>
+        <v>-16666.7</v>
       </c>
       <c r="AJ351" s="5" t="n">
         <v>0</v>
@@ -46020,16 +46016,16 @@
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="3" t="n">
-        <v>3816</v>
+        <v>2315</v>
       </c>
       <c r="B352" s="4" t="s">
-        <v>220</v>
+        <v>82</v>
       </c>
       <c r="C352" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D352" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E352" s="3" t="s">
         <v>151</v>
@@ -46058,11 +46054,11 @@
         <v>0</v>
       </c>
       <c r="M352" s="6" t="n">
-        <v>16196.904</v>
+        <v>0</v>
       </c>
       <c r="N352" s="7" t="n">
         <f aca="false">M352-L352</f>
-        <v>16196.904</v>
+        <v>0</v>
       </c>
       <c r="O352" s="5" t="n">
         <v>0</v>
@@ -46118,21 +46114,21 @@
         <v>0</v>
       </c>
       <c r="AE352" s="6" t="n">
-        <v>51.494</v>
+        <v>0</v>
       </c>
       <c r="AF352" s="7" t="n">
         <f aca="false">AE352-AD352</f>
-        <v>51.494</v>
+        <v>0</v>
       </c>
       <c r="AG352" s="5" t="n">
         <v>0</v>
       </c>
       <c r="AH352" s="6" t="n">
-        <v>16145.41</v>
+        <v>0</v>
       </c>
       <c r="AI352" s="7" t="n">
         <f aca="false">AH352-AG352</f>
-        <v>16145.41</v>
+        <v>0</v>
       </c>
       <c r="AJ352" s="5" t="n">
         <v>0</v>
@@ -46147,7 +46143,7 @@
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="3" t="n">
-        <v>4615</v>
+        <v>3816</v>
       </c>
       <c r="B353" s="4" t="s">
         <v>220</v>
@@ -46182,14 +46178,14 @@
         <v>0</v>
       </c>
       <c r="L353" s="5" t="n">
-        <v>16695.34</v>
+        <v>0</v>
       </c>
       <c r="M353" s="6" t="n">
-        <v>12932.09</v>
+        <v>16196.904</v>
       </c>
       <c r="N353" s="7" t="n">
         <f aca="false">M353-L353</f>
-        <v>-3763.25</v>
+        <v>16196.904</v>
       </c>
       <c r="O353" s="5" t="n">
         <v>0</v>
@@ -46245,42 +46241,42 @@
         <v>0</v>
       </c>
       <c r="AE353" s="6" t="n">
-        <v>17.88</v>
+        <v>51.494</v>
       </c>
       <c r="AF353" s="7" t="n">
         <f aca="false">AE353-AD353</f>
-        <v>17.88</v>
+        <v>51.494</v>
       </c>
       <c r="AG353" s="5" t="n">
-        <v>16695.34</v>
+        <v>0</v>
       </c>
       <c r="AH353" s="6" t="n">
-        <v>12847.89</v>
+        <v>16145.41</v>
       </c>
       <c r="AI353" s="7" t="n">
         <f aca="false">AH353-AG353</f>
-        <v>-3847.45</v>
+        <v>16145.41</v>
       </c>
       <c r="AJ353" s="5" t="n">
         <v>0</v>
       </c>
       <c r="AK353" s="6" t="n">
-        <v>66.32</v>
+        <v>0</v>
       </c>
       <c r="AL353" s="7" t="n">
         <f aca="false">AK353-AJ353</f>
-        <v>66.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="3" t="n">
-        <v>4214</v>
+        <v>4615</v>
       </c>
       <c r="B354" s="4" t="s">
         <v>220</v>
       </c>
       <c r="C354" s="3" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D354" s="3" t="s">
         <v>55</v>
@@ -46309,14 +46305,14 @@
         <v>0</v>
       </c>
       <c r="L354" s="5" t="n">
-        <v>7.76</v>
+        <v>16695.34</v>
       </c>
       <c r="M354" s="6" t="n">
-        <v>11235.03</v>
+        <v>12932.09</v>
       </c>
       <c r="N354" s="7" t="n">
         <f aca="false">M354-L354</f>
-        <v>11227.27</v>
+        <v>-3763.25</v>
       </c>
       <c r="O354" s="5" t="n">
         <v>0</v>
@@ -46372,31 +46368,31 @@
         <v>0</v>
       </c>
       <c r="AE354" s="6" t="n">
-        <v>0</v>
+        <v>17.88</v>
       </c>
       <c r="AF354" s="7" t="n">
         <f aca="false">AE354-AD354</f>
-        <v>0</v>
+        <v>17.88</v>
       </c>
       <c r="AG354" s="5" t="n">
-        <v>7.76</v>
+        <v>16695.34</v>
       </c>
       <c r="AH354" s="6" t="n">
-        <v>11235.03</v>
+        <v>12847.89</v>
       </c>
       <c r="AI354" s="7" t="n">
         <f aca="false">AH354-AG354</f>
-        <v>11227.27</v>
+        <v>-3847.45</v>
       </c>
       <c r="AJ354" s="5" t="n">
         <v>0</v>
       </c>
       <c r="AK354" s="6" t="n">
-        <v>0</v>
+        <v>66.32</v>
       </c>
       <c r="AL354" s="7" t="n">
         <f aca="false">AK354-AJ354</f>
-        <v>0</v>
+        <v>66.32</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -86572,7 +86568,7 @@
       <c r="AL671" s="7"/>
     </row>
     <row r="673" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A673" s="10"/>
+      <c r="A673" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AL670"/>

</xml_diff>